<commit_message>
update BOM list, add gerber file
29/12
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Board_C22\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\git\Board_C22beta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB08F454-435F-4A36-9EAC-708EFF6DFD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049D8AEF-8B5D-47F2-A65E-181EDD6C0E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4476" yWindow="1248" windowWidth="17280" windowHeight="8964" xr2:uid="{3FAD41D8-E8B7-49E3-BAB4-42990604BCD0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3FAD41D8-E8B7-49E3-BAB4-42990604BCD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="100">
   <si>
     <t>NAME</t>
   </si>
@@ -105,18 +105,6 @@
     <t>1 Led nguồn 3V3(nên chọn màu vàng), 1 Led nguồn 5V(đỏ), 4 led hiệu ứng (tùy giới tính)</t>
   </si>
   <si>
-    <t xml:space="preserve">Led RGB </t>
-  </si>
-  <si>
-    <t>https://www.thegioiic.com/products?search=led+rgb+5mm</t>
-  </si>
-  <si>
-    <t>5mm</t>
-  </si>
-  <si>
-    <t>Chung âm hay dương đều được tránh loại chớp 7 màu tự động</t>
-  </si>
-  <si>
     <t>STM32F042F6P6</t>
   </si>
   <si>
@@ -159,9 +147,6 @@
     <t>Module LCD STT7735</t>
   </si>
   <si>
-    <t>Module Joystick</t>
-  </si>
-  <si>
     <t>Module MPU 6050</t>
   </si>
   <si>
@@ -231,18 +216,9 @@
     <t>https://www.thegioiic.com/products/nut-nhan-6x6mm-cao-5mm-4-chan-xuyen-lo</t>
   </si>
   <si>
-    <t>Tatical Buttons SMD</t>
-  </si>
-  <si>
-    <t>https://www.thegioiic.com/products/cong-tac-dip-switch-dan-smd-4-bit-2-54mm</t>
-  </si>
-  <si>
     <t>2.54mm</t>
   </si>
   <si>
-    <t>Dip switch SMD 4 bit</t>
-  </si>
-  <si>
     <t>LM7805</t>
   </si>
   <si>
@@ -313,6 +289,42 @@
   </si>
   <si>
     <t>https://www.thegioiic.com/products/mss-22d18-cong-tac-truot-6-chan-xuyen-lo-on-on-2p2t-0-5a</t>
+  </si>
+  <si>
+    <t>Joystick TH</t>
+  </si>
+  <si>
+    <t>Joystick PS2 Nút Nhấn Điện Trở, Di chuyển: tới, lùi, trái, phải, nút nhấn (thegioiic.com)</t>
+  </si>
+  <si>
+    <t>Tatical Buttons TH</t>
+  </si>
+  <si>
+    <t>Dip switch  4 bit</t>
+  </si>
+  <si>
+    <t>Công Tắc 4 Bit Dip Switch Xuyên Lỗ 2.54mm Màu Đỏ, Khoảng cách chân 2.54mm, 24VDC 25mA (thegioiic.com)</t>
+  </si>
+  <si>
+    <t>2 pin</t>
+  </si>
+  <si>
+    <t>Domino</t>
+  </si>
+  <si>
+    <t>3.5mm</t>
+  </si>
+  <si>
+    <t>KF350-2-V Domino 2 Chân Thẳng 3.5mm Hàn PCB, 300V 10A (thegioiic.com)</t>
+  </si>
+  <si>
+    <t>Capacitor TH</t>
+  </si>
+  <si>
+    <t>100uF-80V</t>
+  </si>
+  <si>
+    <t>Tụ Hoá 100uF 80V 10x25mm Xuyên Lỗ Nichicon, 20%, size(DxL) 10x25mm (thegioiic.com)</t>
   </si>
 </sst>
 </file>
@@ -684,24 +696,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172848C8-5269-4A8B-8868-2550E369E33B}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1"/>
-    <col min="5" max="5" width="23.77734375" customWidth="1"/>
-    <col min="6" max="6" width="96.6640625" customWidth="1"/>
-    <col min="7" max="7" width="62.77734375" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="96.7109375" customWidth="1"/>
+    <col min="7" max="7" width="62.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -724,7 +736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -741,7 +753,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -758,9 +770,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -778,43 +790,43 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -828,7 +840,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -845,29 +857,29 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
       <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
         <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -876,318 +888,331 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11">
+        <v>5525</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12">
-        <v>5525</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>40</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" t="s">
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>43</v>
       </c>
-      <c r="D14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>44</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="D20" t="s">
         <v>45</v>
       </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>91</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="D22" t="s">
         <v>63</v>
       </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>64</v>
       </c>
-      <c r="G18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19">
-        <v>5</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20">
-        <v>3</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>68</v>
       </c>
-      <c r="D22" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
         <v>71</v>
       </c>
-      <c r="D23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="D25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>72</v>
       </c>
-      <c r="B24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" t="s">
-        <v>79</v>
-      </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E26" t="s">
         <v>12</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>84</v>
       </c>
-      <c r="G26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" t="s">
-        <v>70</v>
-      </c>
-      <c r="E27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" s="1" t="s">
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" t="s">
-        <v>83</v>
-      </c>
-      <c r="F28" s="1" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" s="1" t="s">
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>92</v>
-      </c>
-      <c r="E30">
-        <v>5</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>94</v>
       </c>
+      <c r="B31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" t="s">
+        <v>95</v>
+      </c>
       <c r="E31">
         <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1197,28 +1222,30 @@
     <hyperlink ref="F4" r:id="rId3" xr:uid="{192A5693-F55D-401F-9A97-8CB971F2C20F}"/>
     <hyperlink ref="F7" r:id="rId4" xr:uid="{4866CF94-5DC4-49B6-A5FC-678822F94DD3}"/>
     <hyperlink ref="F8" r:id="rId5" xr:uid="{08D33F2E-4418-4195-B48F-55CC4EFC082D}"/>
-    <hyperlink ref="F9" r:id="rId6" xr:uid="{37F5033F-2012-42DD-86B0-04C78073F871}"/>
-    <hyperlink ref="F10" r:id="rId7" xr:uid="{CD1EC580-1620-48D6-8808-75020C446313}"/>
-    <hyperlink ref="F11" r:id="rId8" xr:uid="{DBDFAF4B-9A67-4690-AB40-E7FCAEBD8AAF}"/>
-    <hyperlink ref="F12" r:id="rId9" xr:uid="{6E1759B7-3C87-4C02-BDD0-A35F592DDC6C}"/>
-    <hyperlink ref="F19" r:id="rId10" xr:uid="{EAB123E2-2580-4C27-9FD4-B4ABAED98A21}"/>
-    <hyperlink ref="F21" r:id="rId11" xr:uid="{5844D1AA-F032-4BC2-9769-5EF2EF04C0E6}"/>
-    <hyperlink ref="F20" r:id="rId12" xr:uid="{009801BA-BD54-42F3-B798-B8CB2D73EEDF}"/>
-    <hyperlink ref="F18" r:id="rId13" xr:uid="{8AA535D9-AE40-4D2E-8F64-AE6850DDED7E}"/>
-    <hyperlink ref="F22" r:id="rId14" xr:uid="{C76D2477-FC39-4912-9F82-71EDBFB4F52C}"/>
-    <hyperlink ref="F23" r:id="rId15" xr:uid="{E52E3B74-BBF2-4830-A5EC-87BFC02E49D9}"/>
-    <hyperlink ref="F24" r:id="rId16" xr:uid="{2BDED6A5-2B50-42EE-BB1A-72E8AFDFFE94}"/>
-    <hyperlink ref="F5" r:id="rId17" xr:uid="{79E6A022-E066-45F8-BE97-1B3BF1E6A694}"/>
-    <hyperlink ref="F6" r:id="rId18" xr:uid="{CFCEC254-9C03-43C2-AC60-DFB87B239D95}"/>
-    <hyperlink ref="F26" r:id="rId19" xr:uid="{5EF42469-243D-443E-8DD2-479489028E2D}"/>
-    <hyperlink ref="F27" r:id="rId20" xr:uid="{AAEFEFCE-5FC0-494F-BDE5-63407F2B8EF5}"/>
-    <hyperlink ref="F28" r:id="rId21" xr:uid="{DDCE4A4D-EFAF-4158-920D-607A5212794D}"/>
-    <hyperlink ref="F29" r:id="rId22" xr:uid="{0FF4EEAD-A48A-4AF2-80C3-3E4BE0B3733B}"/>
-    <hyperlink ref="F25" r:id="rId23" xr:uid="{DB0B20D3-D3FF-46ED-A83A-5694CA945431}"/>
-    <hyperlink ref="F30" r:id="rId24" xr:uid="{ACFC5853-949F-4C70-9D15-F5196E870367}"/>
-    <hyperlink ref="F31" r:id="rId25" xr:uid="{23B83868-50A6-4F86-975A-E26B495B9465}"/>
+    <hyperlink ref="F9" r:id="rId6" xr:uid="{CD1EC580-1620-48D6-8808-75020C446313}"/>
+    <hyperlink ref="F10" r:id="rId7" xr:uid="{DBDFAF4B-9A67-4690-AB40-E7FCAEBD8AAF}"/>
+    <hyperlink ref="F11" r:id="rId8" xr:uid="{6E1759B7-3C87-4C02-BDD0-A35F592DDC6C}"/>
+    <hyperlink ref="F18" r:id="rId9" xr:uid="{EAB123E2-2580-4C27-9FD4-B4ABAED98A21}"/>
+    <hyperlink ref="F20" r:id="rId10" xr:uid="{5844D1AA-F032-4BC2-9769-5EF2EF04C0E6}"/>
+    <hyperlink ref="F19" r:id="rId11" xr:uid="{009801BA-BD54-42F3-B798-B8CB2D73EEDF}"/>
+    <hyperlink ref="F17" r:id="rId12" xr:uid="{8AA535D9-AE40-4D2E-8F64-AE6850DDED7E}"/>
+    <hyperlink ref="F21" r:id="rId13" xr:uid="{C76D2477-FC39-4912-9F82-71EDBFB4F52C}"/>
+    <hyperlink ref="F23" r:id="rId14" xr:uid="{2BDED6A5-2B50-42EE-BB1A-72E8AFDFFE94}"/>
+    <hyperlink ref="F5" r:id="rId15" xr:uid="{79E6A022-E066-45F8-BE97-1B3BF1E6A694}"/>
+    <hyperlink ref="F6" r:id="rId16" xr:uid="{CFCEC254-9C03-43C2-AC60-DFB87B239D95}"/>
+    <hyperlink ref="F25" r:id="rId17" xr:uid="{5EF42469-243D-443E-8DD2-479489028E2D}"/>
+    <hyperlink ref="F26" r:id="rId18" xr:uid="{AAEFEFCE-5FC0-494F-BDE5-63407F2B8EF5}"/>
+    <hyperlink ref="F27" r:id="rId19" xr:uid="{DDCE4A4D-EFAF-4158-920D-607A5212794D}"/>
+    <hyperlink ref="F28" r:id="rId20" xr:uid="{0FF4EEAD-A48A-4AF2-80C3-3E4BE0B3733B}"/>
+    <hyperlink ref="F24" r:id="rId21" xr:uid="{DB0B20D3-D3FF-46ED-A83A-5694CA945431}"/>
+    <hyperlink ref="F29" r:id="rId22" xr:uid="{ACFC5853-949F-4C70-9D15-F5196E870367}"/>
+    <hyperlink ref="F30" r:id="rId23" xr:uid="{23B83868-50A6-4F86-975A-E26B495B9465}"/>
+    <hyperlink ref="F14" r:id="rId24" display="https://www.thegioiic.com/products/joystick-ps2-nut-nhan-dien-tro" xr:uid="{CEBF4FA3-6337-4F37-989C-DF2433A7CB8C}"/>
+    <hyperlink ref="F22" r:id="rId25" display="https://www.thegioiic.com/products/cong-tac-4-bit-dip-switch-xuyen-lo-2-54mm-mau-do" xr:uid="{9F60C14A-887A-470B-8072-B431A1AFD881}"/>
+    <hyperlink ref="F31" r:id="rId26" display="https://www.thegioiic.com/products/kf350-2-v-domino-2-chan-thang-3-5mm-han-pcb" xr:uid="{4B87EBBD-F32A-4378-96E1-0E503E9B11F7}"/>
+    <hyperlink ref="F32" r:id="rId27" display="https://www.thegioiic.com/products/tu-hoa-100uf-80v-10x25mm-xuyen-lo-nichicon" xr:uid="{69080FDC-9C55-4AEC-9EEC-74DD1BD70520}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId26"/>
+  <pageSetup orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>